<commit_message>
Modification du document plan test et ajout de commentaires
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spart\Documents\GitHub\JonathanBinot_5_25022021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CB5DDE-0050-4ADD-A28D-786233F4926A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB94A891-CE9B-4BE0-B5E8-3EFB408DD8F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1D66CEF9-EE62-4792-A9B5-A6E822CB7761}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D66CEF9-EE62-4792-A9B5-A6E822CB7761}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -1664,6 +1664,9 @@
   </si>
   <si>
     <t>Un problème pourrait survenir sur cette page si l'id de la commande n'était pas correctement enregistré par l'API. L'id apparaîtrait alors comme undefined</t>
+  </si>
+  <si>
+    <t>Le message pourrait rester affiché malgré un panier rempli, ou bien ne pas s'afficher avec un panier vide</t>
   </si>
 </sst>
 </file>
@@ -1794,7 +1797,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1810,6 +1813,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1852,31 +1861,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2193,23 +2202,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83A0E75-BCCE-4D77-AAC1-046A2BC4E49B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="42.44140625" customWidth="1"/>
-    <col min="5" max="5" width="44.109375" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="5" width="57.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2229,14 +2241,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2249,14 +2261,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -2269,14 +2281,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2289,14 +2301,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -2309,14 +2321,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -2329,14 +2341,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -2349,14 +2361,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -2369,14 +2381,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>99</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -2389,14 +2401,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -2409,14 +2421,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -2429,14 +2441,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -2449,14 +2461,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -2469,14 +2481,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -2485,16 +2497,18 @@
       <c r="E14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="15" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2507,14 +2521,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>101</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -2527,14 +2541,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="11" t="s">
         <v>82</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -2547,7 +2561,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2567,7 +2581,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -2587,14 +2601,14 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="8" t="s">
         <v>96</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -2607,14 +2621,14 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>106</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -2627,14 +2641,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>111</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -2647,14 +2661,14 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>116</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -2669,7 +2683,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>